<commit_message>
Geräte eingepflegt aber es dürfte noch etwas nicht ganz passen
</commit_message>
<xml_diff>
--- a/Pinbelegung.xlsx
+++ b/Pinbelegung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markus\Documents\Arduino\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07354E8C-6425-4110-9EC6-113F539C19B8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB19A434-9967-4B3E-99B0-B5E614161CD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="351">
   <si>
     <t>Hardwaredokumentation von Markus Dreiling geschrieben am 21.09.2019</t>
   </si>
@@ -1055,6 +1055,36 @@
   </si>
   <si>
     <t>,S11_0061</t>
+  </si>
+  <si>
+    <t>Dezimal</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>0x21</t>
+  </si>
+  <si>
+    <t>0x22</t>
+  </si>
+  <si>
+    <t>0x23</t>
+  </si>
+  <si>
+    <t>0x24</t>
+  </si>
+  <si>
+    <t>0x3F</t>
+  </si>
+  <si>
+    <t>UhrModul</t>
+  </si>
+  <si>
+    <t>0x57 und 0x68 zumindest laut i2c Scanner</t>
   </si>
 </sst>
 </file>
@@ -1449,48 +1479,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.734375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1501,7 +1531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1512,7 +1542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1523,7 +1553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1534,7 +1564,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1545,7 +1575,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1556,7 +1586,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1567,7 +1597,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1578,7 +1608,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1589,7 +1619,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1600,7 +1630,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1611,7 +1641,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1622,7 +1652,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1630,7 +1660,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1644,7 +1674,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1655,7 +1685,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1666,7 +1696,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -1677,7 +1707,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1688,7 +1718,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1699,386 +1729,439 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D28" t="s">
+        <v>341</v>
+      </c>
+      <c r="E28" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>46</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D29">
+        <v>32</v>
+      </c>
+      <c r="E29" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>47</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D30">
+        <v>33</v>
+      </c>
+      <c r="E30" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>48</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D31">
+        <v>34</v>
+      </c>
+      <c r="E31" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>49</v>
       </c>
       <c r="C32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32">
+        <v>35</v>
+      </c>
+      <c r="E32" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>50</v>
       </c>
       <c r="C33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33">
+        <v>36</v>
+      </c>
+      <c r="E33" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>51</v>
       </c>
       <c r="C34" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="D34">
+        <v>63</v>
+      </c>
+      <c r="E34" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>349</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
         <v>56</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
         <v>58</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
         <v>64</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
         <v>1</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
         <v>2</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
         <v>3</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
         <v>4</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
         <v>5</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
         <v>6</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
         <v>7</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
         <v>8</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
         <v>9</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
         <v>10</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
         <v>11</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
         <v>12</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
         <v>13</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
         <v>14</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
         <v>15</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
         <v>16</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
         <v>17</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
         <v>18</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66">
         <v>19</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67">
         <v>20</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68">
         <v>21</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69">
         <v>22</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70">
         <v>23</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71">
         <v>24</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72">
         <v>25</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73">
         <v>26</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74">
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76">
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77">
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78">
         <v>31</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79">
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80">
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81">
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82">
         <v>35</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A82">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83">
         <v>36</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A83">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84">
         <v>37</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A84">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85">
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A85">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86">
         <v>39</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A86">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87">
         <v>40</v>
       </c>
     </row>
@@ -2096,17 +2179,17 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.90625" customWidth="1"/>
+    <col min="1" max="1" width="17.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -2114,7 +2197,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -2122,7 +2205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -2130,7 +2213,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>99</v>
       </c>
@@ -2138,7 +2221,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -2146,7 +2229,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -2154,7 +2237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>103</v>
       </c>
@@ -2162,7 +2245,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -2170,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>106</v>
       </c>
@@ -2178,7 +2261,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -2186,27 +2269,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>112</v>
       </c>
@@ -2220,19 +2303,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C6C004-3347-4EEF-9BC7-F9395ACFC7AA}">
   <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" t="str">
         <f>_xlfn.CONCAT(B2:B62)</f>
         <v>,S11_0001,S11_0002,S11_0003,S11_0004,S11_0005,S11_0006,S11_0007,S11_0008,S11_0009,S11_0010,S11_0011,S11_0012,S11_0013,S11_0014,S11_0015,S11_0016,S11_0017,S11_0018,S11_0019,S11_0020,S11_0021,S11_0022,S11_0023,S11_0024,S11_0025,S11_0026,S11_0027,S11_0028,S11_0029,S11_0030,S11_0031,S11_0032,S11_0033,S11_0034,S11_0035,S11_0036,S11_0037,S11_0038,S11_0039,S11_0040,S11_0041,S11_0042,S11_0043,S11_0044,S11_0045,S11_0046,S11_0047,S11_0048,S11_0049,S11_0050,S11_0051,S11_0052,S11_0053,S11_0054,S11_0055,S11_0056,S11_0057,S11_0058,S11_0059,S11_0060,S11_0061</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -2244,7 +2327,7 @@
         <v>,S10_0025,S10_0026,S10_0027,S10_0028,S10_0029,S10_0030,S10_0031,S10_0032,S10_0033,S10_0034,S10_0035,S10_0036,S10_0037,S10_0038,S10_0039,S10_0040,S10_0041,S10_0042,S10_0043,S10_0044,S10_0045,S10_0046,S10_0047,S10_0048,S10_0049,S10_0050,S10_0051,S10_0052,S10_0053,S10_0054,S10_0055,S10_0056,S10_0057,S10_0058,S10_0059,S10_0060,S10_0061,S10_0062,S10_0063,S10_0064,S10_0065,S10_0066,S10_0067,S10_0068,S10_0069,S10_0070,S10_0071,S10_0072,S10_0073,S10_0074,S10_0075,S10_0076,S10_0077,S10_0078,S10_0079,S10_0080,S10_0081,S10_0082,S10_0083,S10_0084,S10_0085,S10_0086,S10_0087,S10_0088,S10_0089,S10_0090,S10_0091,S10_0092,S10_0093,S10_0094,S10_0095,S10_0096,S10_0097,S10_0098,S10_0099,S10_0100,S10_0101,S10_0102,S10_0103,S10_0104,S10_0105,S10_0106,S10_0107,S10_0108,S10_0109,S10_0110,S10_0111,S10_0112,S10_0113,S10_0114,S10_0115,S10_0116,S10_0117,S10_0118,S10_0119,S10_0120,S10_0121,S10_0122,S10_0123</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -2252,7 +2335,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -2260,7 +2343,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -2268,7 +2351,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -2299,7 +2382,7 @@
         <v xml:space="preserve">  const char S11_0001[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -2333,7 +2416,7 @@
         <v xml:space="preserve">  const char S11_0002[] PROGMEM = "Adresse für Sensor 1";</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -2364,7 +2447,7 @@
         <v xml:space="preserve">  const char S11_0003[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -2398,7 +2481,7 @@
         <v xml:space="preserve">  const char S11_0004[] PROGMEM = "Adresse für Sensor 2";</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -2429,7 +2512,7 @@
         <v xml:space="preserve">  const char S11_0005[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -2463,7 +2546,7 @@
         <v xml:space="preserve">  const char S11_0006[] PROGMEM = "Adresse für Sensor 3";</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -2494,7 +2577,7 @@
         <v xml:space="preserve">  const char S11_0007[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -2528,7 +2611,7 @@
         <v xml:space="preserve">  const char S11_0008[] PROGMEM = "Adresse für Sensor 4";</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -2559,7 +2642,7 @@
         <v xml:space="preserve">  const char S11_0009[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -2593,7 +2676,7 @@
         <v xml:space="preserve">  const char S11_0010[] PROGMEM = "Adresse für Sensor 5";</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -2624,7 +2707,7 @@
         <v xml:space="preserve">  const char S11_0011[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -2658,7 +2741,7 @@
         <v xml:space="preserve">  const char S11_0012[] PROGMEM = "Adresse für Sensor 6";</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -2689,7 +2772,7 @@
         <v xml:space="preserve">  const char S11_0013[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -2723,7 +2806,7 @@
         <v xml:space="preserve">  const char S11_0014[] PROGMEM = "Adresse für Sensor 7";</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -2754,7 +2837,7 @@
         <v xml:space="preserve">  const char S11_0015[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -2788,7 +2871,7 @@
         <v xml:space="preserve">  const char S11_0016[] PROGMEM = "Adresse für Sensor 8";</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -2819,7 +2902,7 @@
         <v xml:space="preserve">  const char S11_0017[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -2853,7 +2936,7 @@
         <v xml:space="preserve">  const char S11_0018[] PROGMEM = "Adresse für Sensor 9";</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -2884,7 +2967,7 @@
         <v xml:space="preserve">  const char S11_0019[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -2918,7 +3001,7 @@
         <v xml:space="preserve">  const char S11_0020[] PROGMEM = "Adresse für Sensor 10";</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -2949,7 +3032,7 @@
         <v xml:space="preserve">  const char S11_0021[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -2983,7 +3066,7 @@
         <v xml:space="preserve">  const char S11_0022[] PROGMEM = "Adresse für Sensor 11";</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -3014,7 +3097,7 @@
         <v xml:space="preserve">  const char S11_0023[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -3048,7 +3131,7 @@
         <v xml:space="preserve">  const char S11_0024[] PROGMEM = "Adresse für Sensor 12";</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -3079,7 +3162,7 @@
         <v xml:space="preserve">  const char S11_0025[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -3113,7 +3196,7 @@
         <v xml:space="preserve">  const char S11_0026[] PROGMEM = "Adresse für Sensor 13";</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -3144,7 +3227,7 @@
         <v xml:space="preserve">  const char S11_0027[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -3178,7 +3261,7 @@
         <v xml:space="preserve">  const char S11_0028[] PROGMEM = "Adresse für Sensor 14";</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -3209,7 +3292,7 @@
         <v xml:space="preserve">  const char S11_0029[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -3243,7 +3326,7 @@
         <v xml:space="preserve">  const char S11_0030[] PROGMEM = "Adresse für Sensor 15";</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -3274,7 +3357,7 @@
         <v xml:space="preserve">  const char S11_0031[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -3308,7 +3391,7 @@
         <v xml:space="preserve">  const char S11_0032[] PROGMEM = "Adresse für Sensor 16";</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -3339,7 +3422,7 @@
         <v xml:space="preserve">  const char S11_0033[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -3373,7 +3456,7 @@
         <v xml:space="preserve">  const char S11_0034[] PROGMEM = "Adresse für Sensor 17";</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3404,7 +3487,7 @@
         <v xml:space="preserve">  const char S11_0035[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -3438,7 +3521,7 @@
         <v xml:space="preserve">  const char S11_0036[] PROGMEM = "Adresse für Sensor 18";</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -3469,7 +3552,7 @@
         <v xml:space="preserve">  const char S11_0037[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>155</v>
       </c>
@@ -3503,7 +3586,7 @@
         <v xml:space="preserve">  const char S11_0038[] PROGMEM = "Adresse für Sensor 19";</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>156</v>
       </c>
@@ -3534,7 +3617,7 @@
         <v xml:space="preserve">  const char S11_0039[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>157</v>
       </c>
@@ -3568,7 +3651,7 @@
         <v xml:space="preserve">  const char S11_0040[] PROGMEM = "Adresse für Sensor 20";</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>158</v>
       </c>
@@ -3599,7 +3682,7 @@
         <v xml:space="preserve">  const char S11_0041[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>159</v>
       </c>
@@ -3633,7 +3716,7 @@
         <v xml:space="preserve">  const char S11_0042[] PROGMEM = "Adresse für Sensor 21";</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>160</v>
       </c>
@@ -3664,7 +3747,7 @@
         <v xml:space="preserve">  const char S11_0043[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>161</v>
       </c>
@@ -3698,7 +3781,7 @@
         <v xml:space="preserve">  const char S11_0044[] PROGMEM = "Adresse für Sensor 22";</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>162</v>
       </c>
@@ -3729,7 +3812,7 @@
         <v xml:space="preserve">  const char S11_0045[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>163</v>
       </c>
@@ -3763,7 +3846,7 @@
         <v xml:space="preserve">  const char S11_0046[] PROGMEM = "Adresse für Sensor 23";</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>164</v>
       </c>
@@ -3794,7 +3877,7 @@
         <v xml:space="preserve">  const char S11_0047[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>165</v>
       </c>
@@ -3828,7 +3911,7 @@
         <v xml:space="preserve">  const char S11_0048[] PROGMEM = "Adresse für Sensor 24";</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>166</v>
       </c>
@@ -3859,7 +3942,7 @@
         <v xml:space="preserve">  const char S11_0049[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>167</v>
       </c>
@@ -3893,7 +3976,7 @@
         <v xml:space="preserve">  const char S11_0050[] PROGMEM = "Adresse für Sensor 25";</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>168</v>
       </c>
@@ -3924,7 +4007,7 @@
         <v xml:space="preserve">  const char S11_0051[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>169</v>
       </c>
@@ -3958,7 +4041,7 @@
         <v xml:space="preserve">  const char S11_0052[] PROGMEM = "Adresse für Sensor 26";</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>170</v>
       </c>
@@ -3989,7 +4072,7 @@
         <v xml:space="preserve">  const char S11_0053[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>171</v>
       </c>
@@ -4023,7 +4106,7 @@
         <v xml:space="preserve">  const char S11_0054[] PROGMEM = "Adresse für Sensor 27";</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>172</v>
       </c>
@@ -4054,7 +4137,7 @@
         <v xml:space="preserve">  const char S11_0055[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>173</v>
       </c>
@@ -4088,7 +4171,7 @@
         <v xml:space="preserve">  const char S11_0056[] PROGMEM = "Adresse für Sensor 28";</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>174</v>
       </c>
@@ -4119,7 +4202,7 @@
         <v xml:space="preserve">  const char S11_0057[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>175</v>
       </c>
@@ -4150,7 +4233,7 @@
         <v xml:space="preserve">  const char S11_0058[] PROGMEM = "Adresse für Sensor 29";</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>176</v>
       </c>
@@ -4178,7 +4261,7 @@
         <v xml:space="preserve">  const char S11_0059[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>177</v>
       </c>
@@ -4209,7 +4292,7 @@
         <v xml:space="preserve">  const char S11_0060[] PROGMEM = "Adresse für Sensor 30";</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>178</v>
       </c>
@@ -4237,7 +4320,7 @@
         <v xml:space="preserve">  const char S11_0061[] PROGMEM = "10";</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>179</v>
       </c>
@@ -4268,167 +4351,167 @@
         <v xml:space="preserve">  const char S11_0062[] PROGMEM = "Adresse für Sensor 31";</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>212</v>
       </c>

</xml_diff>